<commit_message>
Updated script and dependencies version
</commit_message>
<xml_diff>
--- a/SeleniumPOM/src/test/resources/testdata/TestData.xlsx
+++ b/SeleniumPOM/src/test/resources/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nads\git\SeleniumPOM\SeleniumPOM\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74B8892-8959-4D3B-A4C2-66C5F3DCA96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA49A3C3-F866-452D-A249-648B9FF1BB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{28CCC827-B3A3-4C69-B2D4-D20A654DE369}"/>
+    <workbookView xWindow="4290" yWindow="1410" windowWidth="19575" windowHeight="12555" activeTab="2" xr2:uid="{28CCC827-B3A3-4C69-B2D4-D20A654DE369}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>Flag</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>Home Page - Place Order</t>
+  </si>
+  <si>
+    <t>AddToBasket</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -169,13 +175,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -705,34 +712,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F76FFFCB-0445-4AEB-9293-14CA3DBBA228}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>